<commit_message>
fix order for admin panel
</commit_message>
<xml_diff>
--- a/Import-template/products.xlsx
+++ b/Import-template/products.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zinmarkyaw/Desktop/ktk-pharmacy/Import-template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\ktk-pharmacy\manage-context\Import-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E7F579-DC0F-8741-980F-81ADAC16539A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="29400" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
+  <calcPr calcId="152511" forceFullCalc="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>product_code</t>
   </si>
@@ -48,9 +47,6 @@
   </si>
   <si>
     <t>packaging</t>
-  </si>
-  <si>
-    <t>mou</t>
   </si>
   <si>
     <t>availability</t>
@@ -813,13 +809,19 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>uom</t>
+  </si>
+  <si>
+    <t>name_mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -982,7 +984,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1017,7 +1019,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1225,30 +1227,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="60" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1256,542 +1258,605 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" ht="60" customHeight="1">
       <c r="A2" s="4">
         <v>44103</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="8">
         <v>7</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="60" customHeight="1">
       <c r="A3" s="4">
         <v>44040</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="8">
         <v>8</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="60" customHeight="1">
       <c r="A4" s="4">
         <v>85007</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4">
         <v>5</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="L4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="60" customHeight="1">
       <c r="A5" s="4">
         <v>85013</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="8">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="8">
         <v>8</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="L5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="6"/>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="60" customHeight="1">
       <c r="A6" s="4">
         <v>85015</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="8">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="8">
         <v>8</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>2</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="L6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="6"/>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="60" customHeight="1">
       <c r="A7" s="4">
         <v>85016</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="8">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="8">
         <v>8</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>2</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="L7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="6"/>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="60" customHeight="1">
       <c r="A8" s="4">
         <v>85017</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="8">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="8">
         <v>7</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="L8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="6"/>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="60" customHeight="1">
       <c r="A9" s="4">
         <v>87007</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="8">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="8">
         <v>7</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>3</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="60" customHeight="1">
       <c r="A10" s="4">
         <v>87008</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="8">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="8">
         <v>8</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>3</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="60" customHeight="1">
       <c r="A11" s="4">
         <v>85019</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="8">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="8">
         <v>8</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>3</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="L11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J11" s="6"/>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="60" customHeight="1">
       <c r="A12" s="4">
         <v>85020</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="8">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="8">
         <v>5</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>4</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="L12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="6"/>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="60" customHeight="1">
       <c r="A13" s="4">
         <v>85073</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="8">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="8">
         <v>5</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>4</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="L13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="6"/>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="60" customHeight="1">
       <c r="A14" s="4">
         <v>85021</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="8">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="8">
         <v>6</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>4</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="L14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J14" s="6"/>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="60" customHeight="1">
       <c r="A15" s="4">
         <v>85022</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="8">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="8">
         <v>6</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15" s="6"/>
-      <c r="L15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="60" customHeight="1">
       <c r="A16" s="4">
         <v>45028</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="8">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="8">
         <v>7</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="60" customHeight="1">
       <c r="A17" s="4">
         <v>45029</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="8">
+        <v>26</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="8">
         <v>7</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>2</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="60" customHeight="1">
       <c r="A18" s="4">
         <v>77343</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="8">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="8">
         <v>9</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>2</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="60" customHeight="1">
       <c r="A19" s="4">
         <v>66089</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="8">
+        <v>28</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="8">
         <v>9</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>3</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="60" customHeight="1">
       <c r="A20" s="4">
         <v>110003</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" s="8">
+        <v>29</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="8">
         <v>9</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>3</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="60" customHeight="1">
       <c r="A21" s="4">
         <v>17011</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="8">
+        <v>30</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="8">
         <v>9</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>4</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="L21">
+      <c r="J21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21">
         <v>1</v>
       </c>
     </row>

</xml_diff>